<commit_message>
Final version send to Diego
</commit_message>
<xml_diff>
--- a/Datos/Resultados Víctor 17112020.xlsx
+++ b/Datos/Resultados Víctor 17112020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabio/Documents/3-Recherche/2020/Univ-Vigo/Datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52ABC56B-01DE-4C4D-9CB0-3F009703FBA6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D219777-3087-FB45-9F11-1244983F02A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21600" yWindow="0" windowWidth="21600" windowHeight="18960" xr2:uid="{86C81D46-EBB6-457F-AE77-808B26C2AFB0}"/>
+    <workbookView xWindow="3600" yWindow="460" windowWidth="21600" windowHeight="17540" activeTab="1" xr2:uid="{86C81D46-EBB6-457F-AE77-808B26C2AFB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Resultados" sheetId="2" r:id="rId1"/>
@@ -473,16 +473,16 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1787,39 +1787,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20837ECF-EB7B-418D-A18F-C5E712D656F3}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17" t="s">
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17" t="s">
+      <c r="H1" s="19"/>
+      <c r="I1" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17" t="s">
+      <c r="J1" s="19"/>
+      <c r="K1" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
     </row>
     <row r="2" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
+      <c r="A2" s="20"/>
       <c r="B2" s="11" t="s">
         <v>82</v>
       </c>
@@ -2055,7 +2055,7 @@
       <c r="K7" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="L7" s="17" t="s">
         <v>42</v>
       </c>
       <c r="M7" s="5" t="s">
@@ -2137,7 +2137,7 @@
       <c r="K9" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="L9" s="20" t="s">
+      <c r="L9" s="18" t="s">
         <v>53</v>
       </c>
       <c r="M9" s="5" t="s">
@@ -2178,10 +2178,10 @@
       <c r="K10" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="L10" s="5" t="s">
+      <c r="L10" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="M10" s="5" t="s">
+      <c r="M10" s="17" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2219,7 +2219,7 @@
       <c r="K11" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="L11" s="19" t="s">
+      <c r="L11" s="17" t="s">
         <v>58</v>
       </c>
       <c r="M11" s="5" t="s">
@@ -2260,7 +2260,7 @@
       <c r="K12" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="L12" s="19" t="s">
+      <c r="L12" s="17" t="s">
         <v>51</v>
       </c>
       <c r="M12" s="5" t="s">
@@ -2818,10 +2818,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51F4E3C1-ADF7-41C1-985B-03747114A9D6}">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2829,7 +2829,7 @@
     <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -2849,7 +2849,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
@@ -2872,8 +2872,12 @@
         <f>+C2/$C$7</f>
         <v>6.9358493491766789E-3</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J2">
+        <f>SUM(C2:C6)</f>
+        <v>4617459</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -2897,7 +2901,7 @@
         <v>1.0828466479074314E-6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
@@ -2921,7 +2925,7 @@
         <v>0.99093397472505984</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
@@ -2945,7 +2949,7 @@
         <v>2.2090071617311599E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
@@ -2969,7 +2973,7 @@
         <v>2.1070030074982799E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>19</v>
       </c>
@@ -2983,7 +2987,7 @@
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
     </row>
-    <row r="10" spans="1:8" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>0</v>
       </c>
@@ -3003,7 +3007,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>6</v>
       </c>
@@ -3027,7 +3031,7 @@
         <v>1.4373607006810743E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
@@ -3051,7 +3055,7 @@
         <v>3.9571420106505493E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
@@ -3075,7 +3079,7 @@
         <v>0.99116551179134449</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
@@ -3099,7 +3103,7 @@
         <v>9.9383225589948568E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>17</v>
       </c>
@@ -3123,7 +3127,7 @@
         <v>7.4305681446841416E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>19</v>
       </c>

</xml_diff>